<commit_message>
updating the config and the testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/applicationTestData_280923.xlsx
+++ b/src/test/resources/testData/applicationTestData_280923.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b7192f114fb507c/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{3C4F5923-F686-4394-9A91-2BFD61A8D2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CB999A7-08DC-4CA3-8A6F-BFA7FE4F97FC}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{3C4F5923-F686-4394-9A91-2BFD61A8D2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F75345F7-0043-43C1-8036-8D50C2C4453E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{0F6E352F-E34F-478D-A787-F3401148C54F}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Firstname</t>
   </si>
@@ -104,28 +104,22 @@
     <t>test12345</t>
   </si>
   <si>
-    <t>Ayesha</t>
-  </si>
-  <si>
-    <t>Yusuf</t>
-  </si>
-  <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>test4@gmail.com</t>
-  </si>
-  <si>
-    <t>test5@gmail.com</t>
-  </si>
-  <si>
     <t>hello123</t>
+  </si>
+  <si>
+    <t>test6@gmail.com</t>
+  </si>
+  <si>
+    <t>test7@gmail.com</t>
+  </si>
+  <si>
+    <t>test8@gmail.com</t>
+  </si>
+  <si>
+    <t>test9@gmail.com</t>
+  </si>
+  <si>
+    <t>test10@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -229,6 +223,10 @@
 </file>
 
 <file path=xl/persons/person16.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person17.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -564,7 +562,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,19 +596,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -618,19 +616,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -638,19 +636,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -658,19 +656,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -678,19 +676,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>

</xml_diff>